<commit_message>
Generate model answer with AI
</commit_message>
<xml_diff>
--- a/AIGradingModel/OCR_Model/Final_SBERT_Dataset.xlsx
+++ b/AIGradingModel/OCR_Model/Final_SBERT_Dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\OCR_Grading_Modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadaf\OneDrive\Nada\FCAI\GP\Scanscore\Scanscore\AIGradingModel\OCR_Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ED4B31-8ADE-4148-8A4E-AE9A78DA3B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D93BE49-D902-4463-8548-D03C8559E5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExamQuestions (Copy)" sheetId="3" r:id="rId1"/>
@@ -315,19 +315,19 @@
     <t>Final Grade</t>
   </si>
   <si>
-    <t>/content/images/WhatsApp Image 2024-04-28 at 4.27.06 PM.jpeg</t>
-  </si>
-  <si>
-    <t>/content/images/WhatsApp Image 2024-04-28 at 4.21.33 PM.jpeg</t>
-  </si>
-  <si>
-    <t>/content/images/WhatsApp Image 2024-04-28 at 4.20.17 PM.jpeg</t>
-  </si>
-  <si>
-    <t>/content/images/WhatsApp Image 2024-04-28 at 4.18.53 PM.jpeg</t>
-  </si>
-  <si>
-    <t>/content/images/WhatsApp Image 2024-04-28 at 4.17.26 PM.jpeg</t>
+    <t>images/WhatsApp Image 2024-04-28 at 4.27.06 PM.jpeg</t>
+  </si>
+  <si>
+    <t>images/WhatsApp Image 2024-04-28 at 4.21.33 PM.jpeg</t>
+  </si>
+  <si>
+    <t>images/WhatsApp Image 2024-04-28 at 4.20.17 PM.jpeg</t>
+  </si>
+  <si>
+    <t>images/WhatsApp Image 2024-04-28 at 4.18.53 PM.jpeg</t>
+  </si>
+  <si>
+    <t>images/WhatsApp Image 2024-04-28 at 4.17.26 PM.jpeg</t>
   </si>
 </sst>
 </file>
@@ -824,16 +824,16 @@
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="8"/>
+    <col min="2" max="2" width="33.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -847,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -861,7 +861,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -873,7 +873,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -887,7 +887,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -899,7 +899,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -913,7 +913,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -925,7 +925,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -937,7 +937,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -949,7 +949,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -961,7 +961,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -973,7 +973,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -985,7 +985,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -997,7 +997,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:3" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1101,16 +1101,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="9.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>90</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1417,16 +1417,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="34.9" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="13.88671875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>67</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1462,17 +1462,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>93</v>
       </c>
@@ -1483,27 +1483,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1521,13 +1521,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>

</xml_diff>